<commit_message>
added all the 9 test cases
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/Login Test data.xlsx
+++ b/src/main/java/TestData/Login Test data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubh\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DA7375-3891-4C1A-A2F4-8D829EC05573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD79BF1-3E01-4BA5-8BC7-5BAB2DCACCDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9DD64F77-DBB6-45E2-A9DB-B21D8E97F984}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Actual</t>
   </si>
@@ -49,13 +49,19 @@
     <t>Expected</t>
   </si>
   <si>
-    <t>Kamla@29</t>
-  </si>
-  <si>
-    <t>Login Successful</t>
-  </si>
-  <si>
     <t>Login Unsuccessful</t>
+  </si>
+  <si>
+    <t>a3jKkxQB</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>Login Unsuccessful with email and password required error</t>
+  </si>
+  <si>
+    <t>id@email.com</t>
   </si>
 </sst>
 </file>
@@ -420,9 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376BBD6D-4D64-4213-A82E-89D6A5A4303E}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -448,50 +452,49 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{2B4F2195-B4D8-43B9-8924-45E107D83461}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{3C9CD3D0-D00F-49AE-AD6F-5D052C3130D7}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{DF183507-7E05-4903-9868-CC84E9E9D681}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{E3502EA6-12EF-41C4-A56C-7C067BD32431}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DF183507-7E05-4903-9868-CC84E9E9D681}"/>
+    <hyperlink ref="B3" r:id="rId2" display="Kamla@29" xr:uid="{E3502EA6-12EF-41C4-A56C-7C067BD32431}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{F06BC638-8C55-45B5-ACE4-7022DCEDD346}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>